<commit_message>
Awaiting of ending of edititng xlsx file
</commit_message>
<xml_diff>
--- a/UniSpreadsheets/Assets/Testing/Sample.xlsx
+++ b/UniSpreadsheets/Assets/Testing/Sample.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Local\GIT\UniSpreadsheets\UniSpreadsheets\Assets\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F57ECDC6-7123-4935-95FD-3C47F2C48E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C050ED75-5C0D-4A1E-A2A4-9CE68C7FACA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{A8EF183D-D65E-4C4E-8B09-321D53100D20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{A8EF183D-D65E-4C4E-8B09-321D53100D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
     <sheet name="Localization" sheetId="2" r:id="rId2"/>
+    <sheet name="Character" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -80,13 +81,31 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Name_Key</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>N_NPC_NickFromForest</t>
+  </si>
+  <si>
+    <t>N_NPC_Homeless</t>
+  </si>
+  <si>
+    <t>N_NPC_Stranger</t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +117,33 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -265,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -277,6 +323,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -675,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E485C54F-7543-415D-98C1-24DFB8D4D6D4}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,4 +781,127 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA085A6B-3ADF-4C66-A56C-2CDF49981083}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>50</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <v>50</v>
+      </c>
+      <c r="C9" s="14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[v1.1.0] Data injection on asset import
</commit_message>
<xml_diff>
--- a/UniSpreadsheets/Assets/Testing/Sample.xlsx
+++ b/UniSpreadsheets/Assets/Testing/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Local\GIT\UniSpreadsheets\UniSpreadsheets\Assets\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Fofanius\UniSpreadsheets\UniSpreadsheets\Assets\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C050ED75-5C0D-4A1E-A2A4-9CE68C7FACA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5AE76C-CA3E-4E05-8B30-850623EC5448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{A8EF183D-D65E-4C4E-8B09-321D53100D20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{A8EF183D-D65E-4C4E-8B09-321D53100D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -99,13 +99,58 @@
   </si>
   <si>
     <t>---</t>
+  </si>
+  <si>
+    <t>L_Tooltip_1</t>
+  </si>
+  <si>
+    <t>Подсказка #1</t>
+  </si>
+  <si>
+    <t>Tooltip #1</t>
+  </si>
+  <si>
+    <t>L_Tooltip_2</t>
+  </si>
+  <si>
+    <t>Подсказка #2</t>
+  </si>
+  <si>
+    <t>Tooltip #2</t>
+  </si>
+  <si>
+    <t>L_Tooltip_3</t>
+  </si>
+  <si>
+    <t>Подсказка #3</t>
+  </si>
+  <si>
+    <t>Tooltip #3</t>
+  </si>
+  <si>
+    <t>L_Tooltip_4</t>
+  </si>
+  <si>
+    <t>Подсказка #4</t>
+  </si>
+  <si>
+    <t>Tooltip #4</t>
+  </si>
+  <si>
+    <t>L_Tooltip_5</t>
+  </si>
+  <si>
+    <t>Подсказка #5</t>
+  </si>
+  <si>
+    <t>Tooltip #5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +194,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -163,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -304,6 +356,39 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -311,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -330,6 +415,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -726,10 +814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E485C54F-7543-415D-98C1-24DFB8D4D6D4}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +866,63 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -787,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA085A6B-3ADF-4C66-A56C-2CDF49981083}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[Fix] Data injection issue coused by empty column of spreadsheet
</commit_message>
<xml_diff>
--- a/UniSpreadsheets/Assets/Testing/Sample.xlsx
+++ b/UniSpreadsheets/Assets/Testing/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Fofanius\UniSpreadsheets\UniSpreadsheets\Assets\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9503AC-E342-408A-BC46-43307312A165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F35735-D0B6-4363-9F7A-86085000F625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A8EF183D-D65E-4C4E-8B09-321D53100D20}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Random</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -398,6 +401,45 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -405,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -427,6 +469,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -742,77 +787,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A34932-6960-4D0B-B031-8304317FD9C8}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="19">
+        <v>3</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>15</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>10</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20">
+        <v>4</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20">
+        <v>2</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>30</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20">
+        <v>5.5</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
       <c r="B6" s="9">
         <v>20</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21">
+        <v>2</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="10">
         <v>5</v>
       </c>
     </row>

</xml_diff>